<commit_message>
Viernes por lla tarde
Para continuar desde el Mac
</commit_message>
<xml_diff>
--- a/data/CellCycleBEA.xlsx
+++ b/data/CellCycleBEA.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizgonzalez/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32918B82-6375-0E45-9D88-978534549441}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="1720" yWindow="820" windowWidth="29440" windowHeight="16780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="27072019" sheetId="3" r:id="rId1"/>
@@ -12,10 +18,10 @@
     <sheet name="Cell Cycle" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'27072019'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'27072019'!$A$2:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Cell Cycle'!$A$1:$O$51</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
   <si>
     <t>Sample:</t>
   </si>
@@ -298,36 +304,12 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G1 Mean</t>
-  </si>
-  <si>
-    <t>G1 CV</t>
-  </si>
-  <si>
-    <t>G2 CV</t>
-  </si>
-  <si>
-    <t>belowG1</t>
-  </si>
-  <si>
-    <t>overG2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -373,16 +355,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,14 +718,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32A9F31-73A2-8541-9ACF-F2BFA2A059A9}">
+  <dimension ref="A2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
@@ -751,538 +733,533 @@
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="G2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="3">
         <v>57.9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="3">
         <v>29.1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D3" s="3">
         <v>9.92</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="3">
         <v>51290</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F3" s="3">
         <v>102144</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G3" s="3">
         <v>11.5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H3" s="3">
         <v>8.41</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I3" s="3">
         <v>2.23</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J3" s="3">
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="3">
         <v>51.7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="3">
         <v>33.700000000000003</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="3">
         <v>9.48</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="3">
         <v>27514</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F4" s="3">
         <v>55347</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="3">
         <v>12.6</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H4" s="3">
         <v>12.5</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I4" s="3">
         <v>3.82</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J4" s="3">
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>65.2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>24.3</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="3">
         <v>6.82</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="3">
         <v>35783</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F5" s="3">
         <v>70372</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>8.24</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H5" s="3">
         <v>6.44</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I5" s="3">
         <v>4.01</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J5" s="3">
         <v>0.44</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>64.8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>22.6</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="3">
         <v>9.17</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="3">
         <v>51740</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F6" s="3">
         <v>101756</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="3">
         <v>7.25</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="3">
         <v>2.61</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J6" s="3">
         <v>0.93</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="5">
         <v>62</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>25.2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="5">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="5">
         <v>70200</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>132938</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="5">
         <v>8.35</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H7" s="5">
         <v>6.47</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I7" s="5">
         <v>2.54</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J7" s="5">
         <v>0.96</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B8" s="5">
         <v>65.2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="5">
         <v>20.399999999999999</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="5">
         <v>7.69</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E8" s="5">
         <v>74761</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F8" s="5">
         <v>142105</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G8" s="5">
         <v>10.5</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H8" s="5">
         <v>10.5</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I8" s="5">
         <v>9.84</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J8" s="5">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>73.599999999999994</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>19.8</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="5">
         <v>7.66</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E9" s="5">
         <v>90838</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>170305</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G9" s="5">
         <v>9.9</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H9" s="5">
         <v>9.92</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I9" s="5">
         <v>1.77</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J9" s="5">
         <v>-0.73</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B10" s="5">
         <v>70.3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>10.6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <v>14.5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <v>65603</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <v>125184</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G10" s="5">
         <v>9.0500000000000007</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H10" s="5">
         <v>8.9499999999999993</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I10" s="5">
         <v>6.96</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J10" s="5">
         <v>-0.36</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <v>38</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>20</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>26.3</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="3">
         <v>35208</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <v>68711</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="3">
         <v>9.24</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="3">
         <v>7.39</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I11" s="3">
         <v>1.66</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J11" s="3">
         <v>14.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>67.8</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>25.1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <v>3.08</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E12" s="3">
         <v>53271</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F12" s="3">
         <v>106779</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G12" s="3">
         <v>11.8</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H12" s="3">
         <v>4.67</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I12" s="3">
         <v>4.6500000000000004</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J12" s="3">
         <v>0.38</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>53.7</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>35.200000000000003</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <v>7.59</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E13" s="3">
         <v>52288</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F13" s="3">
         <v>104393</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="3">
         <v>12.3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>5.55</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I13" s="3">
         <v>3.23</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J13" s="3">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>56.9</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <v>30.5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="3">
         <v>8.82</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="3">
         <v>56793</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F14" s="3">
         <v>110640</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G14" s="3">
         <v>11.1</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="3">
         <v>11.1</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I14" s="3">
         <v>5.52</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J14" s="3">
         <v>-0.66</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B15" s="3">
         <v>64.900000000000006</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C15" s="3">
         <v>24.2</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="3">
         <v>9.24</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E15" s="3">
         <v>53036</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F15" s="3">
         <v>102625</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G15" s="3">
         <v>10</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>10</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I15" s="3">
         <v>2.76</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J15" s="3">
         <v>-0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>59</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>24.1</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D16" s="3">
         <v>11.7</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E16" s="3">
         <v>39280</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F16" s="3">
         <v>76013</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G16" s="3">
         <v>6.83</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>5.96</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I16" s="3">
         <v>2.74</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J16" s="3">
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B17" s="6">
         <v>38.299999999999997</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C17" s="6">
         <v>28.8</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="6">
         <v>17.8</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E17" s="6">
         <v>51620</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F17" s="6">
         <v>101473</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G17" s="6">
         <v>11.2</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H17" s="6">
         <v>5.63</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I17" s="6">
         <v>3.06</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J17" s="6">
         <v>13.3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A2:J2" xr:uid="{77942B9D-5264-3843-A8B4-7B2AA124BA7F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
@@ -1292,7 +1269,7 @@
     <col min="8" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1362,7 +1339,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1397,7 +1374,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1432,7 +1409,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1467,7 +1444,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1502,7 +1479,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1537,7 +1514,7 @@
         <v>-0.31</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1572,7 +1549,7 @@
         <v>-1.56</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1607,7 +1584,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1642,7 +1619,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1677,7 +1654,7 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1712,7 +1689,7 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1782,7 +1759,7 @@
         <v>-0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1817,7 +1794,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1852,7 +1829,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1887,7 +1864,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1922,7 +1899,7 @@
         <v>-0.66</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1957,7 +1934,7 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1992,7 +1969,7 @@
         <v>-0.73</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2027,7 +2004,7 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2062,7 +2039,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2097,7 +2074,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2132,7 +2109,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2167,7 +2144,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2202,7 +2179,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2237,7 +2214,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2272,7 +2249,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2307,7 +2284,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -2353,15 +2330,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D27EA8F-CCD5-AC4D-8D14-583C85F5F835}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:M49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
@@ -2381,7 +2358,7 @@
     <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2400,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" hidden="1">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>65</v>
       </c>
@@ -2451,7 +2428,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="16" hidden="1">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>66</v>
       </c>
@@ -2479,7 +2456,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
@@ -2521,7 +2498,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" hidden="1">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -2563,7 +2540,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2605,7 +2582,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16" hidden="1">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>71</v>
       </c>
@@ -2633,7 +2610,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="16" hidden="1">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -2661,7 +2638,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -2703,7 +2680,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16" hidden="1">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2745,7 +2722,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2787,7 +2764,7 @@
         <v>3.28</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2829,7 +2806,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" hidden="1">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2871,7 +2848,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" hidden="1">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>79</v>
       </c>
@@ -2913,7 +2890,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16" hidden="1">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>80</v>
       </c>
@@ -2955,7 +2932,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16" hidden="1">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>85</v>
       </c>
@@ -2997,7 +2974,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -3039,7 +3016,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16" hidden="1">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
@@ -3081,7 +3058,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16" hidden="1">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>76</v>
       </c>
@@ -3123,7 +3100,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16" hidden="1">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>88</v>
       </c>
@@ -3165,7 +3142,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16" hidden="1">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>89</v>
       </c>
@@ -3207,7 +3184,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
@@ -3249,7 +3226,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
@@ -3291,7 +3268,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16" hidden="1">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -3333,7 +3310,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -3375,7 +3352,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16" hidden="1">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>67</v>
       </c>
@@ -3403,7 +3380,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" ht="16" hidden="1">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>68</v>
       </c>
@@ -3431,7 +3408,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
@@ -3473,7 +3450,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16" hidden="1">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -3515,7 +3492,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
@@ -3557,7 +3534,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
@@ -3599,7 +3576,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16" hidden="1">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
@@ -3641,7 +3618,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16" hidden="1">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>69</v>
       </c>
@@ -3669,7 +3646,7 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="1:14" ht="16" hidden="1">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>70</v>
       </c>
@@ -3697,7 +3674,7 @@
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
@@ -3739,7 +3716,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16" hidden="1">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
@@ -3781,7 +3758,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16" hidden="1">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>78</v>
       </c>
@@ -3823,7 +3800,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16" hidden="1">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>81</v>
       </c>
@@ -3865,7 +3842,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16" hidden="1">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>82</v>
       </c>
@@ -3907,7 +3884,7 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16" hidden="1">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>83</v>
       </c>
@@ -3949,7 +3926,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>30</v>
       </c>
@@ -3991,7 +3968,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16" hidden="1">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>11</v>
       </c>
@@ -4033,7 +4010,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16" hidden="1">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>73</v>
       </c>
@@ -4075,7 +4052,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16" hidden="1">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>74</v>
       </c>
@@ -4117,7 +4094,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16" hidden="1">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>86</v>
       </c>
@@ -4159,7 +4136,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16" hidden="1">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>87</v>
       </c>
@@ -4201,7 +4178,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16" hidden="1">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>63</v>
       </c>
@@ -4229,7 +4206,7 @@
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
     </row>
-    <row r="48" spans="1:14" ht="16" hidden="1">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>64</v>
       </c>
@@ -4257,7 +4234,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>36</v>
       </c>
@@ -4299,7 +4276,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16" hidden="1">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>14</v>
       </c>
@@ -4341,7 +4318,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16" hidden="1">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>19</v>
       </c>
@@ -4384,7 +4361,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O51">
+  <autoFilter ref="A1:O51" xr:uid="{50BFD324-B766-F444-89E1-EAF348FF3284}">
     <filterColumn colId="1">
       <filters>
         <filter val="270519"/>
@@ -4395,238 +4372,5 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BB7475F727342439C221FA398CB396E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="399d9bb98c3417917866416f1ec811ee">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3334966a-ea10-4fb2-b0ef-410f7bba25f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="883b1e56f940a4b8339e44eb6ac71fd0" ns2:_="">
-    <xsd:import namespace="3334966a-ea10-4fb2-b0ef-410f7bba25f3"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3334966a-ea10-4fb2-b0ef-410f7bba25f3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DBE5B-AB5D-4221-93EE-0E80D89D334A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3334966a-ea10-4fb2-b0ef-410f7bba25f3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EE2468F-B629-42AA-BEB7-9E04A7FE5F7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2836DAE5-25E5-484F-8F5E-6BE9914DEA13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>